<commit_message>
try one more temp data for automatic deployment
</commit_message>
<xml_diff>
--- a/FacebookPosts2021.xlsx
+++ b/FacebookPosts2021.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tasha/Desktop/NPLF-Dashboard/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah/Documents/CS/NPLF/NPLF-Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC5ACEB-FA1D-334E-84B5-4EC20EEF919E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E31293-F298-F84E-8404-BF7E48109DBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{67224CD1-7AFB-C34D-94E3-603B098DD09B}"/>
   </bookViews>
@@ -131,7 +131,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -173,7 +173,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,7 +491,7 @@
   <dimension ref="A1:AH248"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -601,31 +601,184 @@
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G2" s="2"/>
+      <c r="G2" s="2">
+        <v>44287</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>6</v>
+      </c>
+      <c r="L2">
+        <v>45</v>
+      </c>
+      <c r="M2">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G3" s="2"/>
+      <c r="G3" s="2">
+        <v>44288</v>
+      </c>
+      <c r="I3">
+        <v>33</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3">
+        <v>6</v>
+      </c>
+      <c r="L3">
+        <v>3</v>
+      </c>
+      <c r="M3">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G4" s="2"/>
+      <c r="G4" s="2">
+        <v>44289</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <v>6</v>
+      </c>
+      <c r="L4">
+        <v>32</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G5" s="2"/>
+      <c r="G5" s="2">
+        <v>44290</v>
+      </c>
+      <c r="I5">
+        <v>32</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>6</v>
+      </c>
+      <c r="L5">
+        <v>343</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G6" s="2"/>
+      <c r="G6" s="2">
+        <v>44291</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>6</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G7" s="2"/>
+      <c r="G7" s="2">
+        <v>44292</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <v>6</v>
+      </c>
+      <c r="L7">
+        <v>3432</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G8" s="2"/>
+      <c r="G8" s="2">
+        <v>44293</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8">
+        <v>6</v>
+      </c>
+      <c r="L8">
+        <v>3</v>
+      </c>
+      <c r="M8">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G9" s="2"/>
+      <c r="G9" s="2">
+        <v>44294</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+      <c r="K9">
+        <v>6</v>
+      </c>
+      <c r="L9">
+        <v>3</v>
+      </c>
+      <c r="M9">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G10" s="2"/>
+      <c r="G10" s="2">
+        <v>44295</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10">
+        <v>4</v>
+      </c>
+      <c r="K10">
+        <v>6</v>
+      </c>
+      <c r="L10">
+        <v>3</v>
+      </c>
+      <c r="M10">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="G11" s="2"/>

</xml_diff>

<commit_message>
remove all temp data
</commit_message>
<xml_diff>
--- a/FacebookPosts2021.xlsx
+++ b/FacebookPosts2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah/Documents/CS/NPLF/NPLF-Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E31293-F298-F84E-8404-BF7E48109DBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01553E9-AFC5-CD4E-9FDF-4DAB78745644}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{67224CD1-7AFB-C34D-94E3-603B098DD09B}"/>
+    <workbookView xWindow="9880" yWindow="4060" windowWidth="28040" windowHeight="17440" xr2:uid="{67224CD1-7AFB-C34D-94E3-603B098DD09B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -491,7 +491,7 @@
   <dimension ref="A1:AH248"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -601,184 +601,31 @@
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G2" s="2">
-        <v>44287</v>
-      </c>
-      <c r="I2">
-        <v>4</v>
-      </c>
-      <c r="J2">
-        <v>3</v>
-      </c>
-      <c r="K2">
-        <v>6</v>
-      </c>
-      <c r="L2">
-        <v>45</v>
-      </c>
-      <c r="M2">
-        <v>3</v>
-      </c>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G3" s="2">
-        <v>44288</v>
-      </c>
-      <c r="I3">
-        <v>33</v>
-      </c>
-      <c r="J3">
-        <v>4</v>
-      </c>
-      <c r="K3">
-        <v>6</v>
-      </c>
-      <c r="L3">
-        <v>3</v>
-      </c>
-      <c r="M3">
-        <v>3</v>
-      </c>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G4" s="2">
-        <v>44289</v>
-      </c>
-      <c r="I4">
-        <v>4</v>
-      </c>
-      <c r="J4">
-        <v>5</v>
-      </c>
-      <c r="K4">
-        <v>6</v>
-      </c>
-      <c r="L4">
-        <v>32</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G5" s="2">
-        <v>44290</v>
-      </c>
-      <c r="I5">
-        <v>32</v>
-      </c>
-      <c r="J5">
-        <v>5</v>
-      </c>
-      <c r="K5">
-        <v>6</v>
-      </c>
-      <c r="L5">
-        <v>343</v>
-      </c>
-      <c r="M5">
-        <v>3</v>
-      </c>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G6" s="2">
-        <v>44291</v>
-      </c>
-      <c r="I6">
-        <v>3</v>
-      </c>
-      <c r="J6">
-        <v>5</v>
-      </c>
-      <c r="K6">
-        <v>6</v>
-      </c>
-      <c r="L6">
-        <v>4</v>
-      </c>
-      <c r="M6">
-        <v>23</v>
-      </c>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G7" s="2">
-        <v>44292</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>4</v>
-      </c>
-      <c r="K7">
-        <v>6</v>
-      </c>
-      <c r="L7">
-        <v>3432</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G8" s="2">
-        <v>44293</v>
-      </c>
-      <c r="I8">
-        <v>4</v>
-      </c>
-      <c r="J8">
-        <v>4</v>
-      </c>
-      <c r="K8">
-        <v>6</v>
-      </c>
-      <c r="L8">
-        <v>3</v>
-      </c>
-      <c r="M8">
-        <v>23</v>
-      </c>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G9" s="2">
-        <v>44294</v>
-      </c>
-      <c r="I9">
-        <v>3</v>
-      </c>
-      <c r="J9">
-        <v>4</v>
-      </c>
-      <c r="K9">
-        <v>6</v>
-      </c>
-      <c r="L9">
-        <v>3</v>
-      </c>
-      <c r="M9">
-        <v>3</v>
-      </c>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="G10" s="2">
-        <v>44295</v>
-      </c>
-      <c r="I10">
-        <v>3</v>
-      </c>
-      <c r="J10">
-        <v>4</v>
-      </c>
-      <c r="K10">
-        <v>6</v>
-      </c>
-      <c r="L10">
-        <v>3</v>
-      </c>
-      <c r="M10">
-        <v>3</v>
-      </c>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="G11" s="2"/>

</xml_diff>